<commit_message>
Running a sample done
</commit_message>
<xml_diff>
--- a/Sample/bin/Debug/net6.0/SalesReport.xlsx
+++ b/Sample/bin/Debug/net6.0/SalesReport.xlsx
@@ -2311,7 +2311,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R2b0f05d2be7b416d"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R10f153be61ad4b70"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2341,7 +2341,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R24c8b283030f44d5"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R35c05df02e414703"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2371,7 +2371,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="Rb5dadd5d78344696"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R55460dc1e62b4018"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2401,7 +2401,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R74ea4ba7e49048da"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="Ra83680e7b1844310"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2431,7 +2431,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="Ra2c7d57288b1440d"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R757bd352d4794eca"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2461,7 +2461,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="Raab3e9731a344c44"/>
+          <c:chart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="R6b72f63043cd4f1d"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2481,7 +2481,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rdd0af7a90b894c4b" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Ra9164bf87c5845e8" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -4174,6 +4174,6 @@
   </x:mergeCells>
   <x:pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="landscape"/>
-  <x:drawing r:id="R29004b34e3ea4b15"/>
+  <x:drawing r:id="Rb4aca410e1ee4741"/>
 </x:worksheet>
 </file>
</xml_diff>